<commit_message>
Agregar nuevas rutas para importar datos desde Excel y refactorizar operaciones de base de datos para manejar solicitudes
</commit_message>
<xml_diff>
--- a/storage/templates/import/bulk-data/plantilla-ambientes.xlsx
+++ b/storage/templates/import/bulk-data/plantilla-ambientes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Projects\PyEduVirtual\PyEducaVirtualBackend\storage\templates\import\bulk-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B0B0C3-36C8-41DB-8E60-1EADC3759334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D38A61-DC44-4DD7-96F8-2367F6B36EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FCFA9209-B65C-48F2-AC47-21205B0966F6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
   <si>
     <t>iEstadoAmbId</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>TUTOR</t>
+  </si>
+  <si>
+    <t>AULA 102</t>
   </si>
 </sst>
 </file>
@@ -302,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -362,11 +365,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -380,6 +403,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -699,30 +731,36 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="18" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="7" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="4" t="s">
         <v>72</v>
       </c>
@@ -784,61 +822,97 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="7">
+        <v>70000001</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7">
+        <v>60</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O3" t="s">
+      <c r="M3" s="7">
+        <v>30</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7">
+        <v>70000002</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="7">
+        <v>60</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O4" t="s">
+      <c r="M4" s="7">
+        <v>30</v>
+      </c>
+      <c r="O4" s="7" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="F1:O1"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:O1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{13BE9D76-EFE4-4C5B-905C-306DA0A81AAF}">
@@ -902,7 +976,7 @@
           <x14:formula1>
             <xm:f>Hoja2!$K$4:$K$14</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D1048576 D3:D1048576</xm:sqref>
+          <xm:sqref>D3:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{315A8537-6ADE-4CDA-A3A7-4E8260E53CC0}">
           <x14:formula1>

</xml_diff>